<commit_message>
varias modificaciones, sobre todo a exploracion_discursos
</commit_message>
<xml_diff>
--- a/Data/datos_base.xlsx
+++ b/Data/datos_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carof\Documents\FORMACION POSGRADO\ditella\MATERIAS\19. taller R Nicolini\Tuits_arg_2019\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CA3249-50AD-470F-9846-B934443EB146}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7E9378-B674-449D-BE28-6210CED3A4B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
   <si>
     <t>Candidato</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>alberto_rsaa</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Presidente</t>
+  </si>
+  <si>
+    <t>Gobernador</t>
   </si>
 </sst>
 </file>
@@ -555,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -568,7 +577,7 @@
     <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -581,8 +590,11 @@
       <c r="D1" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F1" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -595,8 +607,11 @@
       <c r="D2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -609,8 +624,11 @@
       <c r="D3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -623,8 +641,11 @@
       <c r="D4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -637,8 +658,11 @@
       <c r="D5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -651,8 +675,11 @@
       <c r="D6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -665,8 +692,11 @@
       <c r="D7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -679,8 +709,11 @@
       <c r="D8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -693,8 +726,11 @@
       <c r="D9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -707,8 +743,11 @@
       <c r="D10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -721,8 +760,11 @@
       <c r="D11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -735,8 +777,11 @@
       <c r="D12" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -749,8 +794,11 @@
       <c r="D13" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -763,8 +811,11 @@
       <c r="D14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -777,8 +828,11 @@
       <c r="D15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -791,8 +845,11 @@
       <c r="D16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
@@ -805,8 +862,11 @@
       <c r="D17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -819,8 +879,11 @@
       <c r="D18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -833,8 +896,11 @@
       <c r="D19" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
@@ -847,8 +913,11 @@
       <c r="D20" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
@@ -859,8 +928,11 @@
       <c r="D21" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -873,8 +945,11 @@
       <c r="D22" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -886,6 +961,9 @@
       </c>
       <c r="D23" t="s">
         <v>55</v>
+      </c>
+      <c r="F23" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
avance en plteo de temas
</commit_message>
<xml_diff>
--- a/Data/datos_base.xlsx
+++ b/Data/datos_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carof\Documents\FORMACION POSGRADO\ditella\MATERIAS\19. taller R Nicolini\Tuits_arg_2019\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7E9378-B674-449D-BE28-6210CED3A4B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA600E5-0DF4-47A8-A492-97B7F9D58BD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
probando cambiar el sourcing de preparacion_datos_electorales, directo desde git (tablasElectorales)
</commit_message>
<xml_diff>
--- a/Data/datos_base.xlsx
+++ b/Data/datos_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carof\Documents\FORMACION POSGRADO\ditella\MATERIAS\19. taller R Nicolini\Tuits_arg_2019\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA600E5-0DF4-47A8-A492-97B7F9D58BD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0238500A-C242-4715-9D38-4E4FA3AD5719}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -564,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F7"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,7 +577,7 @@
     <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -590,11 +590,11 @@
       <c r="D1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -607,11 +607,11 @@
       <c r="D2" t="s">
         <v>55</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -624,11 +624,11 @@
       <c r="D3" t="s">
         <v>55</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -641,11 +641,11 @@
       <c r="D4" t="s">
         <v>55</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -658,11 +658,11 @@
       <c r="D5" t="s">
         <v>55</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -675,11 +675,11 @@
       <c r="D6" t="s">
         <v>55</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -692,11 +692,11 @@
       <c r="D7" t="s">
         <v>55</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -709,11 +709,11 @@
       <c r="D8" t="s">
         <v>56</v>
       </c>
-      <c r="F8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -726,11 +726,11 @@
       <c r="D9" t="s">
         <v>56</v>
       </c>
-      <c r="F9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -743,11 +743,11 @@
       <c r="D10" t="s">
         <v>56</v>
       </c>
-      <c r="F10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -760,11 +760,11 @@
       <c r="D11" t="s">
         <v>56</v>
       </c>
-      <c r="F11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -777,11 +777,11 @@
       <c r="D12" t="s">
         <v>56</v>
       </c>
-      <c r="F12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -794,11 +794,11 @@
       <c r="D13" t="s">
         <v>56</v>
       </c>
-      <c r="F13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -811,11 +811,11 @@
       <c r="D14" t="s">
         <v>56</v>
       </c>
-      <c r="F14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -828,11 +828,11 @@
       <c r="D15" t="s">
         <v>56</v>
       </c>
-      <c r="F15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -845,11 +845,11 @@
       <c r="D16" t="s">
         <v>55</v>
       </c>
-      <c r="F16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
@@ -862,11 +862,11 @@
       <c r="D17" t="s">
         <v>55</v>
       </c>
-      <c r="F17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -879,11 +879,11 @@
       <c r="D18" t="s">
         <v>55</v>
       </c>
-      <c r="F18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -896,11 +896,11 @@
       <c r="D19" t="s">
         <v>55</v>
       </c>
-      <c r="F19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
@@ -913,11 +913,11 @@
       <c r="D20" t="s">
         <v>55</v>
       </c>
-      <c r="F20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
@@ -928,11 +928,11 @@
       <c r="D21" t="s">
         <v>55</v>
       </c>
-      <c r="F21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -945,11 +945,11 @@
       <c r="D22" t="s">
         <v>55</v>
       </c>
-      <c r="F22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -962,7 +962,7 @@
       <c r="D23" t="s">
         <v>55</v>
       </c>
-      <c r="F23" t="s">
+      <c r="E23" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
borre espacio en nombre
</commit_message>
<xml_diff>
--- a/Data/datos_base.xlsx
+++ b/Data/datos_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carof\Documents\FORMACION POSGRADO\ditella\MATERIAS\19. taller R Nicolini\Tuits_arg_2019\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0238500A-C242-4715-9D38-4E4FA3AD5719}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E4E682-7C04-44BF-8F52-F7E31E281F5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,9 +189,6 @@
     <t>screen_name</t>
   </si>
   <si>
-    <t xml:space="preserve">Raúl Jalil </t>
-  </si>
-  <si>
     <t>Julio Martínez</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>Gobernador</t>
+  </si>
+  <si>
+    <t>Raúl Jalil</t>
   </si>
 </sst>
 </file>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -588,10 +588,10 @@
         <v>30</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -605,10 +605,10 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -622,10 +622,10 @@
         <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -639,10 +639,10 @@
         <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -656,10 +656,10 @@
         <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -673,10 +673,10 @@
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -690,10 +690,10 @@
         <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -707,15 +707,15 @@
         <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -724,10 +724,10 @@
         <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -735,16 +735,16 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -758,10 +758,10 @@
         <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -775,10 +775,10 @@
         <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -792,10 +792,10 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -809,10 +809,10 @@
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -826,10 +826,10 @@
         <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -843,10 +843,10 @@
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -860,10 +860,10 @@
         <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -877,10 +877,10 @@
         <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -894,15 +894,15 @@
         <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>22</v>
@@ -911,10 +911,10 @@
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -926,10 +926,10 @@
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -943,15 +943,15 @@
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>24</v>
@@ -960,10 +960,10 @@
         <v>34</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>